<commit_message>
Alteração slides e adicionar app
</commit_message>
<xml_diff>
--- a/Slides/Cronograma EasyFit.xlsx
+++ b/Slides/Cronograma EasyFit.xlsx
@@ -208,10 +208,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="mmmm/yyyy"/>
     <numFmt numFmtId="166" formatCode="[$R$]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -371,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -552,6 +553,9 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,6 +565,1097 @@
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="Comic Sans MS"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="Comic Sans MS"/>
+              </a:rPr>
+              <a:t>Desempenho do Ticket médio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFB612"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Dezembro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Janeiro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Fevereiro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Folha de cálculo'!$K$12</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1183210694"/>
+        <c:axId val="1227292577"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1183210694"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Comic Sans MS"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Comic Sans MS"/>
+                  </a:rPr>
+                  <a:t>Meses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Comic Sans MS"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1227292577"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1227292577"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Comic Sans MS"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Comic Sans MS"/>
+                  </a:rPr>
+                  <a:t>Valores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Comic Sans MS"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1183210694"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="Comic Sans MS"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Desempenho de n° de vendas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFB612"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Dezembro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Janeiro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Fevereiro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>('Folha de cálculo'!$A$12,'Folha de cálculo'!$E$12,'Folha de cálculo'!$I$12)</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="1180839237"/>
+        <c:axId val="572342635"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1180839237"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Meses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572342635"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="572342635"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Número de vendas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1180839237"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Desempenho do Faturamento</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFB612"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Dezembro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Janeiro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr lvl="0">
+                      <a:defRPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr b="0">
+                        <a:solidFill>
+                          <a:srgbClr val="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Roboto"/>
+                      </a:rPr>
+                      <a:t>Fevereiro</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr lvl="0">
+                    <a:defRPr/>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>('Folha de cálculo'!$C$12,'Folha de cálculo'!$F$12,'Folha de cálculo'!$J$12)</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1204779243"/>
+        <c:axId val="84767764"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1204779243"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Meses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84767764"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84767764"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Valores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1204779243"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -572,7 +1667,83 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4000500" cy="2990850"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Chart 1" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4000500" cy="2990850"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4000500" cy="2990850"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1541,40 +2712,52 @@
         <f>B12/A12</f>
         <v>166.3285714</v>
       </c>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
+      <c r="E12" s="41">
+        <v>12.0</v>
+      </c>
+      <c r="F12" s="74">
+        <v>3900.0</v>
+      </c>
+      <c r="G12" s="74">
+        <v>20.0</v>
+      </c>
+      <c r="I12" s="41">
+        <v>20.0</v>
+      </c>
+      <c r="J12" s="74">
+        <v>4500.0</v>
+      </c>
+      <c r="K12" s="74">
+        <v>300.0</v>
+      </c>
       <c r="L12" s="50"/>
     </row>
     <row r="13">
       <c r="A13" s="60"/>
       <c r="B13" s="42"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
       <c r="L13" s="50"/>
     </row>
     <row r="14">
       <c r="A14" s="60"/>
       <c r="B14" s="42"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
       <c r="L14" s="50"/>
     </row>
     <row r="15">

</xml_diff>